<commit_message>
Summary file fix - add empty cell before description
</commit_message>
<xml_diff>
--- a/clinical_properties_summary.xlsx
+++ b/clinical_properties_summary.xlsx
@@ -10927,35 +10927,71 @@
           <t>Biopsy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>List of Identifiers (separated by commas) of adjacent biospecimens cut from the same sample</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Text term that represents the kind of molecular specimen analyte.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Identifier for the Biospecimen</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>Bone Marrow</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Number of days from the research participant's index date that the biospecimen was obtained.</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>fiducials</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Number of days between the date of sample acquisition and the date that the biospecimen was processed</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Number of days between the date of sample acquisition and the date that the specimen was sectioned</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>Carcinoma in Situ</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Information related to the presence of cells that look abnormal under a microscope but are not cancer. Records the degree of dysplasia for the cyst or lesion under consideration.</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>Fluorescent beads</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>The length of time from beginning to end  required to process or preserve biospecimens in fixative (measured in minutes)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>The field to identify the type of fixative used to preserve a tissue specimen</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr">
         <is>
           <t>Microscope</t>
@@ -10971,21 +11007,61 @@
           <t>Antifade without DAPI</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Numeric value that represents the count of proliferating cells determined during pathologic review of the sample slide(s).</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Parent Identifier from which the biospecimen was obtained. The parent could be another biospecimen or a research participant.</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Numeric value to represent the percentage of cell death in a malignant tumor sample or specimen.</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Numeric value to represent the percentage of normal cell content in a malignant tumor sample or specimen.</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Numeric value to represent the percentage of reactive cells that are present in a malignant tumor sample or specimen but are not malignant such as fibroblasts</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Numeric value to represent the percentage of infiltration by tumor cells in a sample.</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Numeric value to represent the percentage of tumor nuclei in a malignant neoplasm sample or specimen.</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Number of days from the research participant's date of death that the biospecimen was obtained</t>
+        </is>
+      </c>
       <c r="Z3" t="inlineStr">
         <is>
           <t>Frozen</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Identifier that describes the protocol by which the sample was obtained or generated. E.g. Protocols.io</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Numeric value to describe the thickness of a slice to tissue taken from a biospecimen,  measured in microns (um).</t>
+        </is>
+      </c>
       <c r="AC3" t="inlineStr">
         <is>
           <t>Cold Pack</t>
@@ -11011,7 +11087,11 @@
           <t>End of Treatment</t>
         </is>
       </c>
-      <c r="AH3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Number of tumor-infiltrating lymphocytes</t>
+        </is>
+      </c>
       <c r="AI3" t="inlineStr">
         <is>
           <t>Local Tumor Recurrence</t>
@@ -11024,71 +11104,35 @@
           <t>Excision</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>List of Identifiers (separated by commas) of adjacent biospecimens cut from the same sample</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Text term that represents the kind of molecular specimen analyte.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Identifier for the Biospecimen</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>Cell Block</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Number of days from the research participant's index date that the biospecimen was obtained.</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>matrix</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Number of days between the date of sample acquisition and the date that the biospecimen was processed</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Number of days between the date of sample acquisition and the date that the specimen was sectioned</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>Moderate dysplasia</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Information related to the presence of cells that look abnormal under a microscope but are not cancer. Records the degree of dysplasia for the cyst or lesion under consideration.</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>Grid slides (hemocytometer)</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>The length of time from beginning to end  required to process or preserve biospecimens in fixative (measured in minutes)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>The field to identify the type of fixative used to preserve a tissue specimen</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
@@ -11100,57 +11144,17 @@
           <t>Aqueous (water based) medium</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Numeric value that represents the count of proliferating cells determined during pathologic review of the sample slide(s).</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Parent Identifier from which the biospecimen was obtained. The parent could be another biospecimen or a research participant.</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Numeric value to represent the percentage of cell death in a malignant tumor sample or specimen.</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Numeric value to represent the percentage of normal cell content in a malignant tumor sample or specimen.</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Numeric value to represent the percentage of reactive cells that are present in a malignant tumor sample or specimen but are not malignant such as fibroblasts</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>Numeric value to represent the percentage of infiltration by tumor cells in a sample.</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Numeric value to represent the percentage of tumor nuclei in a malignant neoplasm sample or specimen.</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Number of days from the research participant's date of death that the biospecimen was obtained</t>
-        </is>
-      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Identifier that describes the protocol by which the sample was obtained or generated. E.g. Protocols.io</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Numeric value to describe the thickness of a slice to tissue taken from a biospecimen,  measured in microns (um).</t>
-        </is>
-      </c>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr">
         <is>
           <t>Dry Ice</t>
@@ -11176,11 +11180,7 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Number of tumor-infiltrating lymphocytes</t>
-        </is>
-      </c>
+      <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="inlineStr">
         <is>
           <t>Metastatic</t>
@@ -11831,7 +11831,11 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>anatomic location of sample (Procedure site)</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
@@ -11851,11 +11855,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>anatomic location of sample (Procedure site)</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -12040,7 +12040,11 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>anatomic location of sample (Procedure site)</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
@@ -12076,11 +12080,7 @@
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>anatomic location of sample (Procedure site)</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>

</xml_diff>